<commit_message>
Added visualizations of MARS model
</commit_message>
<xml_diff>
--- a/PH_forecasts.xlsx
+++ b/PH_forecasts.xlsx
@@ -653,7 +653,7 @@
         <v>1.48</v>
       </c>
       <c r="AG2" t="n">
-        <v>8.49616861867698</v>
+        <v>8.49616861867697</v>
       </c>
     </row>
     <row r="3">
@@ -754,7 +754,7 @@
         <v>3.04</v>
       </c>
       <c r="AG3" t="n">
-        <v>8.56419965411937</v>
+        <v>8.56419965411936</v>
       </c>
     </row>
     <row r="4">
@@ -956,7 +956,7 @@
         <v>1.48</v>
       </c>
       <c r="AG5" t="n">
-        <v>8.60790810700557</v>
+        <v>8.60790810700558</v>
       </c>
     </row>
     <row r="6">
@@ -1158,7 +1158,7 @@
         <v>1.44</v>
       </c>
       <c r="AG7" t="n">
-        <v>8.55441461485443</v>
+        <v>8.55441461485442</v>
       </c>
     </row>
     <row r="8">
@@ -1259,7 +1259,7 @@
         <v>3.02</v>
       </c>
       <c r="AG8" t="n">
-        <v>8.49620031264027</v>
+        <v>8.49620031264026</v>
       </c>
     </row>
     <row r="9">
@@ -1360,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="AG9" t="n">
-        <v>8.50928521180398</v>
+        <v>8.50928521180397</v>
       </c>
     </row>
     <row r="10">
@@ -1562,7 +1562,7 @@
         <v>3.12</v>
       </c>
       <c r="AG11" t="n">
-        <v>8.76273238353367</v>
+        <v>8.76273238353366</v>
       </c>
     </row>
     <row r="12">
@@ -1764,7 +1764,7 @@
         <v>1.42</v>
       </c>
       <c r="AG13" t="n">
-        <v>8.62251776877967</v>
+        <v>8.62251776877966</v>
       </c>
     </row>
     <row r="14">
@@ -1865,7 +1865,7 @@
         <v>1.46</v>
       </c>
       <c r="AG14" t="n">
-        <v>8.55688502909968</v>
+        <v>8.55688502909967</v>
       </c>
     </row>
     <row r="15">
@@ -1966,7 +1966,7 @@
         <v>1.44</v>
       </c>
       <c r="AG15" t="n">
-        <v>8.53283153848794</v>
+        <v>8.53283153848793</v>
       </c>
     </row>
     <row r="16">
@@ -2067,7 +2067,7 @@
         <v>1.6</v>
       </c>
       <c r="AG16" t="n">
-        <v>8.23893448419654</v>
+        <v>8.23893448419653</v>
       </c>
     </row>
     <row r="17">
@@ -2166,7 +2166,7 @@
         <v>1.6</v>
       </c>
       <c r="AG17" t="n">
-        <v>8.43109304784827</v>
+        <v>8.43109304784826</v>
       </c>
     </row>
     <row r="18">
@@ -2368,7 +2368,7 @@
         <v>1.44</v>
       </c>
       <c r="AG19" t="n">
-        <v>8.50081043572814</v>
+        <v>8.50081043572813</v>
       </c>
     </row>
     <row r="20">
@@ -2570,7 +2570,7 @@
         <v>1.46</v>
       </c>
       <c r="AG21" t="n">
-        <v>8.6134576691491</v>
+        <v>8.61345766914909</v>
       </c>
     </row>
     <row r="22">
@@ -2772,7 +2772,7 @@
         <v>1.36</v>
       </c>
       <c r="AG23" t="n">
-        <v>8.61517814457627</v>
+        <v>8.61517814457626</v>
       </c>
     </row>
     <row r="24">
@@ -2873,7 +2873,7 @@
         <v>3.18</v>
       </c>
       <c r="AG24" t="n">
-        <v>8.56537780739968</v>
+        <v>8.56537780739967</v>
       </c>
     </row>
     <row r="25">
@@ -2974,7 +2974,7 @@
         <v>1.4</v>
       </c>
       <c r="AG25" t="n">
-        <v>8.6965972797388</v>
+        <v>8.69659727973879</v>
       </c>
     </row>
     <row r="26">
@@ -3075,7 +3075,7 @@
         <v>1.4</v>
       </c>
       <c r="AG26" t="n">
-        <v>8.66750845841863</v>
+        <v>8.66750845841862</v>
       </c>
     </row>
     <row r="27">
@@ -3176,7 +3176,7 @@
         <v>1.4</v>
       </c>
       <c r="AG27" t="n">
-        <v>8.48737123813714</v>
+        <v>8.48737123813713</v>
       </c>
     </row>
     <row r="28">
@@ -3378,7 +3378,7 @@
         <v>3.28</v>
       </c>
       <c r="AG29" t="n">
-        <v>8.64579205721826</v>
+        <v>8.64579205721825</v>
       </c>
     </row>
     <row r="30">
@@ -3479,7 +3479,7 @@
         <v>3.24</v>
       </c>
       <c r="AG30" t="n">
-        <v>8.676956283871</v>
+        <v>8.67695628387099</v>
       </c>
     </row>
     <row r="31">
@@ -3580,7 +3580,7 @@
         <v>3.26</v>
       </c>
       <c r="AG31" t="n">
-        <v>8.72722977321333</v>
+        <v>8.72722977321332</v>
       </c>
     </row>
     <row r="32">
@@ -3681,7 +3681,7 @@
         <v>3.28</v>
       </c>
       <c r="AG32" t="n">
-        <v>8.64513895974601</v>
+        <v>8.645138959746</v>
       </c>
     </row>
     <row r="33">
@@ -3782,7 +3782,7 @@
         <v>3.28</v>
       </c>
       <c r="AG33" t="n">
-        <v>8.57476485172312</v>
+        <v>8.57476485172311</v>
       </c>
     </row>
     <row r="34">
@@ -3883,7 +3883,7 @@
         <v>1.5</v>
       </c>
       <c r="AG34" t="n">
-        <v>8.61087099550792</v>
+        <v>8.61087099550791</v>
       </c>
     </row>
     <row r="35">
@@ -4085,7 +4085,7 @@
         <v>1.56</v>
       </c>
       <c r="AG36" t="n">
-        <v>8.66161867343646</v>
+        <v>8.66161867343645</v>
       </c>
     </row>
     <row r="37">
@@ -4186,7 +4186,7 @@
         <v>3</v>
       </c>
       <c r="AG37" t="n">
-        <v>8.4749049649177</v>
+        <v>8.47490496491769</v>
       </c>
     </row>
     <row r="38">
@@ -4287,7 +4287,7 @@
         <v>3.08</v>
       </c>
       <c r="AG38" t="n">
-        <v>8.4245027534265</v>
+        <v>8.42450275342649</v>
       </c>
     </row>
     <row r="39">
@@ -4388,7 +4388,7 @@
         <v>3.06</v>
       </c>
       <c r="AG39" t="n">
-        <v>8.44183870272358</v>
+        <v>8.44183870272357</v>
       </c>
     </row>
     <row r="40">
@@ -4792,7 +4792,7 @@
         <v>1.38</v>
       </c>
       <c r="AG43" t="n">
-        <v>8.67821483461994</v>
+        <v>8.67821483461993</v>
       </c>
     </row>
     <row r="44">
@@ -4893,7 +4893,7 @@
         <v>1.34</v>
       </c>
       <c r="AG44" t="n">
-        <v>8.60064594637534</v>
+        <v>8.60064594637533</v>
       </c>
     </row>
     <row r="45">
@@ -4994,7 +4994,7 @@
         <v>1.38</v>
       </c>
       <c r="AG45" t="n">
-        <v>8.53067924168116</v>
+        <v>8.53067924168115</v>
       </c>
     </row>
     <row r="46">
@@ -5095,7 +5095,7 @@
         <v>1.42</v>
       </c>
       <c r="AG46" t="n">
-        <v>8.61757250967123</v>
+        <v>8.61757250967122</v>
       </c>
     </row>
     <row r="47">
@@ -5196,7 +5196,7 @@
         <v>3.28</v>
       </c>
       <c r="AG47" t="n">
-        <v>8.74257329489248</v>
+        <v>8.74257329489247</v>
       </c>
     </row>
     <row r="48">
@@ -5499,7 +5499,7 @@
         <v>3.1</v>
       </c>
       <c r="AG50" t="n">
-        <v>8.63891431054052</v>
+        <v>8.63891431054051</v>
       </c>
     </row>
     <row r="51">
@@ -5600,7 +5600,7 @@
         <v>3.06</v>
       </c>
       <c r="AG51" t="n">
-        <v>8.661041340629</v>
+        <v>8.66104134062899</v>
       </c>
     </row>
     <row r="52">
@@ -6307,7 +6307,7 @@
         <v>1.32</v>
       </c>
       <c r="AG58" t="n">
-        <v>8.47044841307298</v>
+        <v>8.47044841307297</v>
       </c>
     </row>
     <row r="59">
@@ -6408,7 +6408,7 @@
         <v>1.48</v>
       </c>
       <c r="AG59" t="n">
-        <v>8.60657730469729</v>
+        <v>8.60657730469728</v>
       </c>
     </row>
     <row r="60">
@@ -6509,7 +6509,7 @@
         <v>1.38</v>
       </c>
       <c r="AG60" t="n">
-        <v>8.52335490977044</v>
+        <v>8.52335490977043</v>
       </c>
     </row>
     <row r="61">
@@ -6610,7 +6610,7 @@
         <v>1.42</v>
       </c>
       <c r="AG61" t="n">
-        <v>8.69876617088835</v>
+        <v>8.69876617088834</v>
       </c>
     </row>
     <row r="62">
@@ -6812,7 +6812,7 @@
         <v>1.44</v>
       </c>
       <c r="AG63" t="n">
-        <v>8.65355482781847</v>
+        <v>8.65355482781846</v>
       </c>
     </row>
     <row r="64">
@@ -7115,7 +7115,7 @@
         <v>1.54</v>
       </c>
       <c r="AG66" t="n">
-        <v>8.73255523646473</v>
+        <v>8.73255523646472</v>
       </c>
     </row>
     <row r="67">
@@ -7216,7 +7216,7 @@
         <v>1.5</v>
       </c>
       <c r="AG67" t="n">
-        <v>8.64029698678656</v>
+        <v>8.64029698678655</v>
       </c>
     </row>
     <row r="68">
@@ -7317,7 +7317,7 @@
         <v>1.44</v>
       </c>
       <c r="AG68" t="n">
-        <v>8.60315019257231</v>
+        <v>8.6031501925723</v>
       </c>
     </row>
     <row r="69">
@@ -7721,7 +7721,7 @@
         <v>1.32</v>
       </c>
       <c r="AG72" t="n">
-        <v>8.39962121816934</v>
+        <v>8.39962121816933</v>
       </c>
     </row>
     <row r="73">
@@ -7822,7 +7822,7 @@
         <v>1.42</v>
       </c>
       <c r="AG73" t="n">
-        <v>8.53580348554536</v>
+        <v>8.53580348554535</v>
       </c>
     </row>
     <row r="74">
@@ -7923,7 +7923,7 @@
         <v>3.32</v>
       </c>
       <c r="AG74" t="n">
-        <v>8.60017381171257</v>
+        <v>8.60017381171256</v>
       </c>
     </row>
     <row r="75">
@@ -8024,7 +8024,7 @@
         <v>3.34</v>
       </c>
       <c r="AG75" t="n">
-        <v>8.57894248784737</v>
+        <v>8.57894248784736</v>
       </c>
     </row>
     <row r="76">
@@ -8125,7 +8125,7 @@
         <v>3.26</v>
       </c>
       <c r="AG76" t="n">
-        <v>8.50629860041239</v>
+        <v>8.50629860041238</v>
       </c>
     </row>
     <row r="77">
@@ -8226,7 +8226,7 @@
         <v>3.14</v>
       </c>
       <c r="AG77" t="n">
-        <v>8.47785181145598</v>
+        <v>8.47785181145597</v>
       </c>
     </row>
     <row r="78">
@@ -8327,7 +8327,7 @@
         <v>3.36</v>
       </c>
       <c r="AG78" t="n">
-        <v>8.49028053067406</v>
+        <v>8.49028053067405</v>
       </c>
     </row>
     <row r="79">
@@ -8428,7 +8428,7 @@
         <v>1.36</v>
       </c>
       <c r="AG79" t="n">
-        <v>8.68822947671984</v>
+        <v>8.68822947671983</v>
       </c>
     </row>
     <row r="80">
@@ -8529,7 +8529,7 @@
         <v>3.24</v>
       </c>
       <c r="AG80" t="n">
-        <v>8.6629615695202</v>
+        <v>8.66296156952019</v>
       </c>
     </row>
     <row r="81">
@@ -8731,7 +8731,7 @@
         <v>1.38</v>
       </c>
       <c r="AG82" t="n">
-        <v>8.75646542943854</v>
+        <v>8.75646542943853</v>
       </c>
     </row>
     <row r="83">
@@ -8832,7 +8832,7 @@
         <v>1.26</v>
       </c>
       <c r="AG83" t="n">
-        <v>8.51445688367745</v>
+        <v>8.51445688367744</v>
       </c>
     </row>
     <row r="84">
@@ -9034,7 +9034,7 @@
         <v>1.32</v>
       </c>
       <c r="AG85" t="n">
-        <v>8.51582005395452</v>
+        <v>8.51582005395451</v>
       </c>
     </row>
     <row r="86">
@@ -9135,7 +9135,7 @@
         <v>1.44</v>
       </c>
       <c r="AG86" t="n">
-        <v>8.46739687115288</v>
+        <v>8.46739687115287</v>
       </c>
     </row>
     <row r="87">
@@ -9236,7 +9236,7 @@
         <v>1.42</v>
       </c>
       <c r="AG87" t="n">
-        <v>8.74867498907207</v>
+        <v>8.74867498907206</v>
       </c>
     </row>
     <row r="88">
@@ -9539,7 +9539,7 @@
         <v>2.86</v>
       </c>
       <c r="AG90" t="n">
-        <v>8.47589023165225</v>
+        <v>8.47589023165224</v>
       </c>
     </row>
     <row r="91">
@@ -9741,7 +9741,7 @@
         <v>2.84</v>
       </c>
       <c r="AG92" t="n">
-        <v>8.63301171599718</v>
+        <v>8.63301171599717</v>
       </c>
     </row>
     <row r="93">
@@ -9943,7 +9943,7 @@
         <v>3</v>
       </c>
       <c r="AG94" t="n">
-        <v>8.45559707181284</v>
+        <v>8.45559707181283</v>
       </c>
     </row>
     <row r="95">
@@ -10044,7 +10044,7 @@
         <v>3</v>
       </c>
       <c r="AG95" t="n">
-        <v>8.53110017284363</v>
+        <v>8.53110017284362</v>
       </c>
     </row>
     <row r="96">
@@ -10145,7 +10145,7 @@
         <v>3.28</v>
       </c>
       <c r="AG96" t="n">
-        <v>8.60710123984199</v>
+        <v>8.607101239842</v>
       </c>
     </row>
     <row r="97">
@@ -10448,7 +10448,7 @@
         <v>1.44</v>
       </c>
       <c r="AG99" t="n">
-        <v>8.6832952375979</v>
+        <v>8.68329523759789</v>
       </c>
     </row>
     <row r="100">
@@ -10549,7 +10549,7 @@
         <v>3.04</v>
       </c>
       <c r="AG100" t="n">
-        <v>8.59943632638422</v>
+        <v>8.59943632638421</v>
       </c>
     </row>
     <row r="101">
@@ -10650,7 +10650,7 @@
         <v>3.04</v>
       </c>
       <c r="AG101" t="n">
-        <v>8.58936282703583</v>
+        <v>8.58936282703582</v>
       </c>
     </row>
     <row r="102">
@@ -10751,7 +10751,7 @@
         <v>3.24</v>
       </c>
       <c r="AG102" t="n">
-        <v>8.56513011821391</v>
+        <v>8.5651301182139</v>
       </c>
     </row>
     <row r="103">
@@ -10852,7 +10852,7 @@
         <v>3.1</v>
       </c>
       <c r="AG103" t="n">
-        <v>8.7394798411419</v>
+        <v>8.73947984114188</v>
       </c>
     </row>
     <row r="104">
@@ -11155,7 +11155,7 @@
         <v>1.42</v>
       </c>
       <c r="AG106" t="n">
-        <v>8.77292549420895</v>
+        <v>8.77292549420894</v>
       </c>
     </row>
     <row r="107">
@@ -11559,7 +11559,7 @@
         <v>1.38</v>
       </c>
       <c r="AG110" t="n">
-        <v>8.578192600354</v>
+        <v>8.57819260035399</v>
       </c>
     </row>
     <row r="111">
@@ -11660,7 +11660,7 @@
         <v>1.5</v>
       </c>
       <c r="AG111" t="n">
-        <v>8.62651092008241</v>
+        <v>8.6265109200824</v>
       </c>
     </row>
     <row r="112">
@@ -11761,7 +11761,7 @@
         <v>1.34</v>
       </c>
       <c r="AG112" t="n">
-        <v>8.64088884963143</v>
+        <v>8.64088884963142</v>
       </c>
     </row>
     <row r="113">
@@ -11862,7 +11862,7 @@
         <v>1.34</v>
       </c>
       <c r="AG113" t="n">
-        <v>8.6685202406838</v>
+        <v>8.66852024068379</v>
       </c>
     </row>
     <row r="114">
@@ -11963,7 +11963,7 @@
         <v>3.08</v>
       </c>
       <c r="AG114" t="n">
-        <v>8.69185347372068</v>
+        <v>8.69185347372067</v>
       </c>
     </row>
     <row r="115">
@@ -12165,7 +12165,7 @@
         <v>1.26</v>
       </c>
       <c r="AG116" t="n">
-        <v>8.56392829917042</v>
+        <v>8.56392829917041</v>
       </c>
     </row>
     <row r="117">
@@ -12468,7 +12468,7 @@
         <v>3.16</v>
       </c>
       <c r="AG119" t="n">
-        <v>8.68288198721599</v>
+        <v>8.68288198721598</v>
       </c>
     </row>
     <row r="120">
@@ -12670,7 +12670,7 @@
         <v>1.44</v>
       </c>
       <c r="AG121" t="n">
-        <v>8.64786412959062</v>
+        <v>8.64786412959061</v>
       </c>
     </row>
     <row r="122">
@@ -12771,7 +12771,7 @@
         <v>1.46</v>
       </c>
       <c r="AG122" t="n">
-        <v>8.67496953799546</v>
+        <v>8.67496953799545</v>
       </c>
     </row>
     <row r="123">
@@ -12872,7 +12872,7 @@
         <v>1.38</v>
       </c>
       <c r="AG123" t="n">
-        <v>8.64016097869423</v>
+        <v>8.64016097869422</v>
       </c>
     </row>
     <row r="124">
@@ -13074,7 +13074,7 @@
         <v>1.36</v>
       </c>
       <c r="AG125" t="n">
-        <v>8.55311906231528</v>
+        <v>8.55311906231529</v>
       </c>
     </row>
     <row r="126">
@@ -13678,7 +13678,7 @@
         <v>3.06</v>
       </c>
       <c r="AG131" t="n">
-        <v>8.58463591107726</v>
+        <v>8.58463591107725</v>
       </c>
     </row>
     <row r="132">
@@ -14688,7 +14688,7 @@
         <v>3.08</v>
       </c>
       <c r="AG141" t="n">
-        <v>8.43073043494721</v>
+        <v>8.4307304349472</v>
       </c>
     </row>
     <row r="142">
@@ -15597,7 +15597,7 @@
         <v>1.36</v>
       </c>
       <c r="AG150" t="n">
-        <v>8.44515252295575</v>
+        <v>8.44515252295574</v>
       </c>
     </row>
     <row r="151">
@@ -16203,7 +16203,7 @@
         <v>1.68</v>
       </c>
       <c r="AG156" t="n">
-        <v>8.49351928462793</v>
+        <v>8.49351928462794</v>
       </c>
     </row>
     <row r="157">
@@ -17213,7 +17213,7 @@
         <v>1.3</v>
       </c>
       <c r="AG166" t="n">
-        <v>8.59020318157029</v>
+        <v>8.5902031815703</v>
       </c>
     </row>
     <row r="167">
@@ -17514,7 +17514,7 @@
         <v>3.14</v>
       </c>
       <c r="AG169" t="n">
-        <v>8.66252807148464</v>
+        <v>8.66252807148465</v>
       </c>
     </row>
     <row r="170">
@@ -18019,7 +18019,7 @@
         <v>1.44</v>
       </c>
       <c r="AG174" t="n">
-        <v>8.36400762918133</v>
+        <v>8.36400762918134</v>
       </c>
     </row>
     <row r="175">
@@ -18120,7 +18120,7 @@
         <v>1.42</v>
       </c>
       <c r="AG175" t="n">
-        <v>8.49059664820723</v>
+        <v>8.49059664820722</v>
       </c>
     </row>
     <row r="176">
@@ -18726,7 +18726,7 @@
         <v>1.3</v>
       </c>
       <c r="AG181" t="n">
-        <v>8.48600151743945</v>
+        <v>8.48600151743946</v>
       </c>
     </row>
     <row r="182">
@@ -19130,7 +19130,7 @@
         <v>1.34</v>
       </c>
       <c r="AG185" t="n">
-        <v>8.48477771069127</v>
+        <v>8.48477771069128</v>
       </c>
     </row>
     <row r="186">
@@ -19433,7 +19433,7 @@
         <v>1.84</v>
       </c>
       <c r="AG188" t="n">
-        <v>8.35091198510712</v>
+        <v>8.35091198510711</v>
       </c>
     </row>
     <row r="189">
@@ -19534,7 +19534,7 @@
         <v>3.18</v>
       </c>
       <c r="AG189" t="n">
-        <v>8.60904036283384</v>
+        <v>8.60904036283385</v>
       </c>
     </row>
     <row r="190">
@@ -19938,7 +19938,7 @@
         <v>1.38</v>
       </c>
       <c r="AG193" t="n">
-        <v>8.5483670585446</v>
+        <v>8.54836705854461</v>
       </c>
     </row>
     <row r="194">
@@ -21954,7 +21954,7 @@
         <v>1.48</v>
       </c>
       <c r="AG213" t="n">
-        <v>8.44831522757723</v>
+        <v>8.44831522757724</v>
       </c>
     </row>
     <row r="214">
@@ -22358,7 +22358,7 @@
         <v>3.04</v>
       </c>
       <c r="AG217" t="n">
-        <v>8.32362138062744</v>
+        <v>8.32362138062743</v>
       </c>
     </row>
     <row r="218">
@@ -22964,7 +22964,7 @@
         <v>1.36</v>
       </c>
       <c r="AG223" t="n">
-        <v>8.51546942971386</v>
+        <v>8.51546942971385</v>
       </c>
     </row>
     <row r="224">
@@ -23065,7 +23065,7 @@
         <v>1.36</v>
       </c>
       <c r="AG224" t="n">
-        <v>8.4336534143167</v>
+        <v>8.43365341431669</v>
       </c>
     </row>
     <row r="225">
@@ -23671,7 +23671,7 @@
         <v>1.36</v>
       </c>
       <c r="AG230" t="n">
-        <v>8.42048132627493</v>
+        <v>8.42048132627494</v>
       </c>
     </row>
     <row r="231">
@@ -24376,7 +24376,7 @@
         <v>1.62</v>
       </c>
       <c r="AG237" t="n">
-        <v>8.45089797921902</v>
+        <v>8.45089797921901</v>
       </c>
     </row>
     <row r="238">
@@ -25184,7 +25184,7 @@
         <v>3.34</v>
       </c>
       <c r="AG245" t="n">
-        <v>8.49449434873322</v>
+        <v>8.49449434873321</v>
       </c>
     </row>
     <row r="246">
@@ -25891,7 +25891,7 @@
         <v>1.44</v>
       </c>
       <c r="AG252" t="n">
-        <v>8.36851417562716</v>
+        <v>8.36851417562717</v>
       </c>
     </row>
     <row r="253">
@@ -27200,7 +27200,7 @@
         <v>3.36</v>
       </c>
       <c r="AG265" t="n">
-        <v>8.56257435549179</v>
+        <v>8.5625743554918</v>
       </c>
     </row>
     <row r="266">

</xml_diff>